<commit_message>
TF-92 timestamp 추가, 통계 정보 조회 api 조정
</commit_message>
<xml_diff>
--- a/DB/tools/data.xlsx
+++ b/DB/tools/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bootcamp\Today_Feeling\DB\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JIHOON\Desktop\study\board\Today_Feeling\DB\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ECF9DE-F9FF-4601-B7AC-01D919198440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18CB103-8139-457A-99E4-8F3881AF6A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5805" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,13 +403,10 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C154"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="95.375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -425,6 +422,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>